<commit_message>
trascrizione continua; stima dimensionale aggiornata realisticamente
</commit_message>
<xml_diff>
--- a/Documentazione/Stima Dimensionale.xlsx
+++ b/Documentazione/Stima Dimensionale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BIG-DATA-MANAGEMENT\Documentazione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documenti\Big Data Management Progetto\BIG-DATA-MANAGEMENT\Documentazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC7A5CB-853C-44AF-B0FA-83B4FCF9D6DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96F78D6-383E-424A-B03D-548076E402D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4563AA14-1549-40CC-9750-27BCFC0E19C8}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="173">
   <si>
     <t>Professore/Studente (wp_users)</t>
   </si>
@@ -613,6 +613,9 @@
   </si>
   <si>
     <t>200 ore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totale lezione + contenuto </t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -709,7 +712,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -872,16 +875,16 @@
                   <c:v>2.6530586183071136E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.533378720283508</c:v>
+                  <c:v>6.343156099319458</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.066757440567017</c:v>
+                  <c:v>12.686312198638916</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.600136160850525</c:v>
+                  <c:v>19.029468297958374</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>62.133514881134033</c:v>
+                  <c:v>25.372624397277832</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1759,14 +1762,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>5661660</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>70485</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1827,7 +1830,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2125,20 +2128,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD4317F-1194-4DBE-A226-C8A3F783138C}">
   <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" workbookViewId="0">
+    <sheetView topLeftCell="E13" workbookViewId="0">
       <selection activeCell="I22" sqref="I22:I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2325,7 +2328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I18" s="2" t="s">
         <v>80</v>
       </c>
@@ -2564,7 +2567,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I19" s="2">
         <v>1</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2622,7 +2625,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2635,7 +2638,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2648,31 +2651,31 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I24" s="2" t="s">
         <v>82</v>
       </c>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I25" s="2" t="s">
         <v>83</v>
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I26" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I27" s="2" t="s">
         <v>85</v>
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
@@ -2683,7 +2686,7 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
@@ -2694,7 +2697,7 @@
       </c>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
@@ -2705,7 +2708,7 @@
       </c>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>44</v>
       </c>
@@ -2716,7 +2719,7 @@
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>45</v>
       </c>
@@ -2727,7 +2730,7 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
@@ -2738,7 +2741,7 @@
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>47</v>
       </c>
@@ -2749,7 +2752,7 @@
       </c>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>48</v>
       </c>
@@ -2760,7 +2763,7 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2784,23 +2787,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA74DE-5AFB-4B1A-B5BF-A35F66F07F1A}">
   <dimension ref="A1:AT139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F5"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="29.77734375" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2814,7 +2817,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2832,7 +2835,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>55</v>
       </c>
@@ -2844,14 +2847,14 @@
       </c>
       <c r="F3">
         <f>SUM(D49,D58,D67)</f>
-        <v>3474758</v>
+        <v>1416564</v>
       </c>
       <c r="G3">
         <f>(25+7)*D13</f>
         <v>34880</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>41</v>
       </c>
@@ -2867,10 +2870,10 @@
       </c>
       <c r="G4">
         <f>960*D49</f>
-        <v>2265840000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1309554240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
@@ -2886,14 +2889,14 @@
       </c>
       <c r="G5">
         <f>G4+G3</f>
-        <v>2265874880</v>
+        <v>1309589120</v>
       </c>
       <c r="H5">
         <f>G5/(1024*1024*1024)</f>
-        <v>2.1102604269981384</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.2196499109268188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>43</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>44</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
@@ -2917,7 +2920,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
@@ -2933,7 +2936,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>48</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>49</v>
       </c>
@@ -2949,7 +2952,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>111</v>
       </c>
@@ -2958,12 +2961,12 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>129</v>
@@ -2972,7 +2975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>120</v>
@@ -2981,7 +2984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>130</v>
@@ -2990,7 +2993,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
         <v>131</v>
@@ -2999,7 +3002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>132</v>
@@ -3008,7 +3011,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>133</v>
@@ -3017,7 +3020,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>121</v>
@@ -3026,7 +3029,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22" t="s">
         <v>111</v>
@@ -3036,15 +3039,15 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>56</v>
       </c>
@@ -3083,7 +3086,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>57</v>
       </c>
@@ -3114,7 +3117,7 @@
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
@@ -3145,13 +3148,13 @@
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C30">
-        <f>1024*1024</f>
-        <v>1048576</v>
+        <f>D58+D67</f>
+        <v>52445</v>
       </c>
       <c r="D30" t="s">
         <v>110</v>
@@ -3182,7 +3185,7 @@
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
@@ -3213,7 +3216,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
@@ -3247,7 +3250,7 @@
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
@@ -3278,7 +3281,7 @@
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>63</v>
       </c>
@@ -3309,7 +3312,7 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>64</v>
       </c>
@@ -3340,7 +3343,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>65</v>
       </c>
@@ -3371,7 +3374,7 @@
       <c r="AA36" s="2"/>
       <c r="AB36" s="2"/>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>66</v>
       </c>
@@ -3402,7 +3405,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>67</v>
       </c>
@@ -3433,7 +3436,7 @@
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>68</v>
       </c>
@@ -3464,7 +3467,7 @@
       <c r="AA39" s="2"/>
       <c r="AB39" s="2"/>
     </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>69</v>
       </c>
@@ -3495,7 +3498,7 @@
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
     </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>70</v>
       </c>
@@ -3526,7 +3529,7 @@
       <c r="AA41" s="2"/>
       <c r="AB41" s="2"/>
     </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>71</v>
       </c>
@@ -3558,7 +3561,7 @@
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
     </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>72</v>
       </c>
@@ -3589,7 +3592,7 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>73</v>
       </c>
@@ -3620,7 +3623,7 @@
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>74</v>
       </c>
@@ -3651,7 +3654,7 @@
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>75</v>
       </c>
@@ -3682,7 +3685,7 @@
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>76</v>
       </c>
@@ -3713,7 +3716,7 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>77</v>
       </c>
@@ -3744,13 +3747,13 @@
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>111</v>
       </c>
       <c r="D49">
         <f>SUM(C26:C48)</f>
-        <v>2360250</v>
+        <v>1364119</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -3776,7 +3779,7 @@
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -3804,7 +3807,7 @@
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>135</v>
       </c>
@@ -3835,7 +3838,7 @@
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>136</v>
       </c>
@@ -3866,7 +3869,7 @@
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>137</v>
       </c>
@@ -3897,7 +3900,7 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>138</v>
       </c>
@@ -3928,7 +3931,7 @@
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>124</v>
       </c>
@@ -3959,7 +3962,7 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>139</v>
       </c>
@@ -3990,13 +3993,12 @@
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C57">
-        <f>1024*1024</f>
-        <v>1048576</v>
+        <v>50000</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -4022,11 +4024,11 @@
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="D58">
         <f>SUM(C51:C57)</f>
-        <v>1048645</v>
+        <v>50069</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -4052,7 +4054,7 @@
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>141</v>
       </c>
@@ -4081,7 +4083,7 @@
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>142</v>
       </c>
@@ -4112,7 +4114,7 @@
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>139</v>
       </c>
@@ -4143,7 +4145,7 @@
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>143</v>
       </c>
@@ -4174,12 +4176,12 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="2"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>144</v>
       </c>
       <c r="C63">
-        <v>65535</v>
+        <v>2048</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -4205,7 +4207,7 @@
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>137</v>
       </c>
@@ -4236,7 +4238,7 @@
       <c r="AA64" s="2"/>
       <c r="AB64" s="2"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>145</v>
       </c>
@@ -4267,7 +4269,7 @@
       <c r="AA65" s="2"/>
       <c r="AB65" s="2"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>135</v>
       </c>
@@ -4298,14 +4300,14 @@
       <c r="AA66" s="2"/>
       <c r="AB66" s="2"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" t="s">
         <v>111</v>
       </c>
       <c r="D67">
         <f>SUM(C60:C66)</f>
-        <v>65863</v>
+        <v>2376</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -4331,7 +4333,7 @@
       <c r="AA67" s="2"/>
       <c r="AB67" s="2"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -4360,7 +4362,7 @@
       <c r="AA68" s="2"/>
       <c r="AB68" s="2"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>147</v>
       </c>
@@ -4391,7 +4393,7 @@
       <c r="AA69" s="2"/>
       <c r="AB69" s="2"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>120</v>
       </c>
@@ -4422,7 +4424,7 @@
       <c r="AA70" s="2"/>
       <c r="AB70" s="2"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>148</v>
       </c>
@@ -4453,7 +4455,7 @@
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>149</v>
       </c>
@@ -4484,7 +4486,7 @@
       <c r="AA72" s="2"/>
       <c r="AB72" s="2"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>150</v>
       </c>
@@ -4515,7 +4517,7 @@
       <c r="AA73" s="2"/>
       <c r="AB73" s="2"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B74" s="2"/>
       <c r="C74" t="s">
         <v>111</v>
@@ -4548,7 +4550,7 @@
       <c r="AA74" s="2"/>
       <c r="AB74" s="2"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>151</v>
       </c>
@@ -4577,7 +4579,7 @@
       <c r="AA75" s="2"/>
       <c r="AB75" s="2"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>152</v>
       </c>
@@ -4608,7 +4610,7 @@
       <c r="AA76" s="2"/>
       <c r="AB76" s="2"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>120</v>
       </c>
@@ -4639,7 +4641,7 @@
       <c r="AA77" s="2"/>
       <c r="AB77" s="2"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>111</v>
       </c>
@@ -4671,7 +4673,7 @@
       <c r="AA78" s="2"/>
       <c r="AB78" s="2"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -4699,7 +4701,7 @@
       <c r="AA79" s="2"/>
       <c r="AB79" s="2"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>142</v>
       </c>
@@ -4730,7 +4732,7 @@
       <c r="AA80" s="2"/>
       <c r="AB80" s="2"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>120</v>
       </c>
@@ -4761,7 +4763,7 @@
       <c r="AA81" s="2"/>
       <c r="AB81" s="2"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D82">
         <f>SUM(C80:C81)</f>
         <v>204</v>
@@ -4790,7 +4792,7 @@
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -4818,7 +4820,7 @@
       <c r="AA83" s="2"/>
       <c r="AB83" s="2"/>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>80</v>
       </c>
@@ -4849,7 +4851,7 @@
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>81</v>
       </c>
@@ -4880,7 +4882,7 @@
       <c r="AA85" s="2"/>
       <c r="AB85" s="2"/>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>82</v>
       </c>
@@ -4911,7 +4913,7 @@
       <c r="AA86" s="2"/>
       <c r="AB86" s="2"/>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>83</v>
       </c>
@@ -4942,7 +4944,7 @@
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>84</v>
       </c>
@@ -4973,7 +4975,7 @@
       <c r="AA88" s="2"/>
       <c r="AB88" s="2"/>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>85</v>
       </c>
@@ -5004,7 +5006,7 @@
       <c r="AA89" s="2"/>
       <c r="AB89" s="2"/>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>86</v>
       </c>
@@ -5035,7 +5037,7 @@
       <c r="AA90" s="2"/>
       <c r="AB90" s="2"/>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>87</v>
       </c>
@@ -5066,7 +5068,7 @@
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>88</v>
       </c>
@@ -5097,7 +5099,7 @@
       <c r="AA92" s="2"/>
       <c r="AB92" s="2"/>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>89</v>
       </c>
@@ -5128,7 +5130,7 @@
       <c r="AA93" s="2"/>
       <c r="AB93" s="2"/>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>90</v>
       </c>
@@ -5159,7 +5161,7 @@
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>91</v>
       </c>
@@ -5190,7 +5192,7 @@
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>92</v>
       </c>
@@ -5221,7 +5223,7 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>93</v>
       </c>
@@ -5252,7 +5254,7 @@
       <c r="AA97" s="2"/>
       <c r="AB97" s="2"/>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>94</v>
       </c>
@@ -5283,7 +5285,7 @@
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>111</v>
       </c>
@@ -5315,12 +5317,12 @@
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>119</v>
       </c>
@@ -5328,7 +5330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>120</v>
       </c>
@@ -5336,7 +5338,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>121</v>
       </c>
@@ -5344,7 +5346,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>122</v>
       </c>
@@ -5352,7 +5354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
         <v>111</v>
       </c>
@@ -5361,7 +5363,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -5372,7 +5374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>125</v>
       </c>
@@ -5380,7 +5382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>126</v>
       </c>
@@ -5388,7 +5390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>127</v>
       </c>
@@ -5396,7 +5398,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>119</v>
       </c>
@@ -5404,7 +5406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
         <v>111</v>
       </c>
@@ -5413,7 +5415,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="117" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="117" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -5455,7 +5457,7 @@
       <c r="AS117" s="2"/>
       <c r="AT117" s="2"/>
     </row>
-    <row r="118" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="118" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
@@ -5497,7 +5499,7 @@
       <c r="AS118" s="2"/>
       <c r="AT118" s="2"/>
     </row>
-    <row r="119" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="119" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -5539,7 +5541,7 @@
       <c r="AS119" s="2"/>
       <c r="AT119" s="2"/>
     </row>
-    <row r="120" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="120" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -5581,7 +5583,7 @@
       <c r="AS120" s="2"/>
       <c r="AT120" s="2"/>
     </row>
-    <row r="121" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="121" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -5623,7 +5625,7 @@
       <c r="AS121" s="2"/>
       <c r="AT121" s="2"/>
     </row>
-    <row r="122" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="122" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -5665,7 +5667,7 @@
       <c r="AS122" s="2"/>
       <c r="AT122" s="2"/>
     </row>
-    <row r="123" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="123" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
@@ -5707,7 +5709,7 @@
       <c r="AS123" s="2"/>
       <c r="AT123" s="2"/>
     </row>
-    <row r="124" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="124" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
@@ -5749,7 +5751,7 @@
       <c r="AS124" s="2"/>
       <c r="AT124" s="2"/>
     </row>
-    <row r="125" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="125" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
@@ -5791,7 +5793,7 @@
       <c r="AS125" s="2"/>
       <c r="AT125" s="2"/>
     </row>
-    <row r="126" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="126" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
@@ -5833,7 +5835,7 @@
       <c r="AS126" s="2"/>
       <c r="AT126" s="2"/>
     </row>
-    <row r="127" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="127" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -5875,7 +5877,7 @@
       <c r="AS127" s="2"/>
       <c r="AT127" s="2"/>
     </row>
-    <row r="128" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="128" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -5917,7 +5919,7 @@
       <c r="AS128" s="2"/>
       <c r="AT128" s="2"/>
     </row>
-    <row r="129" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="129" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -5959,7 +5961,7 @@
       <c r="AS129" s="2"/>
       <c r="AT129" s="2"/>
     </row>
-    <row r="130" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="130" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -6001,7 +6003,7 @@
       <c r="AS130" s="2"/>
       <c r="AT130" s="2"/>
     </row>
-    <row r="131" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="131" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
@@ -6043,7 +6045,7 @@
       <c r="AS131" s="2"/>
       <c r="AT131" s="2"/>
     </row>
-    <row r="132" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="132" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
@@ -6085,7 +6087,7 @@
       <c r="AS132" s="2"/>
       <c r="AT132" s="2"/>
     </row>
-    <row r="133" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="133" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
@@ -6127,7 +6129,7 @@
       <c r="AS133" s="2"/>
       <c r="AT133" s="2"/>
     </row>
-    <row r="134" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="134" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
@@ -6169,7 +6171,7 @@
       <c r="AS134" s="2"/>
       <c r="AT134" s="2"/>
     </row>
-    <row r="135" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="135" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
@@ -6211,7 +6213,7 @@
       <c r="AS135" s="2"/>
       <c r="AT135" s="2"/>
     </row>
-    <row r="136" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="136" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
@@ -6253,7 +6255,7 @@
       <c r="AS136" s="2"/>
       <c r="AT136" s="2"/>
     </row>
-    <row r="137" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="137" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
@@ -6295,7 +6297,7 @@
       <c r="AS137" s="2"/>
       <c r="AT137" s="2"/>
     </row>
-    <row r="138" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="138" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
@@ -6337,7 +6339,7 @@
       <c r="AS138" s="2"/>
       <c r="AT138" s="2"/>
     </row>
-    <row r="139" spans="7:46" x14ac:dyDescent="0.3">
+    <row r="139" spans="7:46" x14ac:dyDescent="0.25">
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
@@ -6394,18 +6396,18 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -6413,17 +6415,17 @@
         <v>2700000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -6431,7 +6433,7 @@
         <v>123000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -6451,23 +6453,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A193714-DD7A-459A-8C67-E4D8B240C94F}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.109375" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" customWidth="1"/>
-    <col min="3" max="3" width="83.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" customWidth="1"/>
+    <col min="3" max="3" width="83.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -6479,17 +6481,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -6497,15 +6499,16 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B9">
-        <v>3474758</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <f>1416564+2376</f>
+        <v>1418940</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -6513,7 +6516,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -6521,7 +6524,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -6530,88 +6533,88 @@
         <v>2.6530586183071136E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>169</v>
       </c>
       <c r="B20">
         <f>5*960*B9/(1024*1024*1024)</f>
-        <v>15.533378720283508</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6.343156099319458</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>165</v>
       </c>
       <c r="B24">
         <f>B20+5*960*(B9)/(1024*1024*1024)</f>
-        <v>31.066757440567017</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>12.686312198638916</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>166</v>
       </c>
       <c r="B25">
         <f>B24+960*5*B9/(1024*1024*1024)</f>
-        <v>46.600136160850525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19.029468297958374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>167</v>
       </c>
       <c r="B26">
         <f>B25+B9*5*960/(1024*1024*1024)</f>
-        <v>62.133514881134033</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25.372624397277832</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>168</v>
       </c>
       <c r="B27">
         <f>B9*960/(1024*1024*1024)</f>
-        <v>3.1066757440567017</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1.2686312198638916</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>171</v>
       </c>
       <c r="B28">
         <f>B9*200/(1024*1024*1024)</f>
-        <v>0.64722411334514618</v>
+        <v>0.26429817080497742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>